<commit_message>
Correccion control de errores en archivos importados
</commit_message>
<xml_diff>
--- a/arc/xls/arc_Libro1.xlsx
+++ b/arc/xls/arc_Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvanrivera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2161C97B-2BE3-4230-8BA3-4C87DEDE2799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94A53F0-9A93-453B-BA75-9FA2226EFDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="3030" windowWidth="13350" windowHeight="11385" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
+    <workbookView xWindow="1065" yWindow="2985" windowWidth="13350" windowHeight="11385" xr2:uid="{AC666F3B-5823-41FB-96A7-40BA11624A31}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78ABAF4D-8D4E-4C34-82E1-BB8F60C584FB}">
   <dimension ref="B3:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>